<commit_message>
Completed session and decorator (don't know for decorator)
Did session login and signup succefully, added test cases and tested it,
though for testing signup delete the row already there. Also did
decorator but not sure for that.
</commit_message>
<xml_diff>
--- a/pdTwo/src/main/resources/csv/user.xlsx
+++ b/pdTwo/src/main/resources/csv/user.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27504"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\BL6PEPF0001995F\EXCELCNV\758790af-2830-4a9d-adfd-40b360e2641e\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -102,12 +102,37 @@
   </si>
   <si>
     <t>nonfaculty</t>
+  </si>
+  <si>
+    <t>lifeisgood@gmail.com</t>
+  </si>
+  <si>
+    <t>hopscotch</t>
+  </si>
+  <si>
+    <t>userManagement.Student</t>
+  </si>
+  <si>
+    <t>good@gmail.com</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>notgood@gmail.com</t>
+  </si>
+  <si>
+    <t>hello@gmail.com</t>
+  </si>
+  <si>
+    <t>hello</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="18">
     <font>
       <sz val="11"/>
@@ -942,7 +967,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1048,6 +1073,86 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6">
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Delete User method added
Added a delete user method that works and added that to run before the
test cases each time for signing up successfully. May need to organize
it, probably move open workbook to another method.
</commit_message>
<xml_diff>
--- a/pdTwo/src/main/resources/csv/user.xlsx
+++ b/pdTwo/src/main/resources/csv/user.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>name</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>hello</t>
+  </si>
+  <si>
+    <t>helloworld@gmail.com</t>
+  </si>
+  <si>
+    <t>helloworld</t>
   </si>
 </sst>
 </file>
@@ -967,7 +973,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1153,6 +1159,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="13">
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Merged Session into User
Basically added functionality of session into user, and tweaked it up a
lot for it to work. You sign up with userId, email, password, and class.
Login with email and password. Logging in with previous stuff may not
work though cause of different cell types then data types being inputed.
</commit_message>
<xml_diff>
--- a/pdTwo/src/main/resources/csv/user.xlsx
+++ b/pdTwo/src/main/resources/csv/user.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="47">
   <si>
     <t>name</t>
   </si>
@@ -132,6 +132,51 @@
   </si>
   <si>
     <t>helloworld</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>helloworld1@gmail.com</t>
+  </si>
+  <si>
+    <t>helloworld1</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>hell@gmail.com</t>
+  </si>
+  <si>
+    <t>hell</t>
+  </si>
+  <si>
+    <t>helloworld2@gmail.com</t>
+  </si>
+  <si>
+    <t>helloworld2</t>
+  </si>
+  <si>
+    <t>helloworld3@gmail.com</t>
+  </si>
+  <si>
+    <t>helloworld3</t>
+  </si>
+  <si>
+    <t>helloworld4@gmail.com</t>
+  </si>
+  <si>
+    <t>helloworld4</t>
+  </si>
+  <si>
+    <t>helloworld5@gmail.com</t>
+  </si>
+  <si>
+    <t>helloworld5</t>
   </si>
 </sst>
 </file>
@@ -973,7 +1018,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1173,6 +1218,162 @@
         <v>0</v>
       </c>
     </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="n">
+        <v>-3.0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="n">
+        <v>-4.0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="n">
+        <v>-5.0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Validation in Login implemented, plus update tests
Yeah, added 3 lines and changed an == to equalsignorecase in the user
class, changed accesstest to test for the changes, added another test
case, etc...
</commit_message>
<xml_diff>
--- a/pdTwo/src/main/resources/csv/user.xlsx
+++ b/pdTwo/src/main/resources/csv/user.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="54">
   <si>
     <t>name</t>
   </si>
@@ -177,6 +177,27 @@
   </si>
   <si>
     <t>helloworld5</t>
+  </si>
+  <si>
+    <t>helloworld6@gmail.com</t>
+  </si>
+  <si>
+    <t>helloworld6</t>
+  </si>
+  <si>
+    <t>Visitor</t>
+  </si>
+  <si>
+    <t>helloworld7@gmail.com</t>
+  </si>
+  <si>
+    <t>helloworld7</t>
+  </si>
+  <si>
+    <t>helloworld8@gmail.com</t>
+  </si>
+  <si>
+    <t>helloworld8</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1039,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1374,6 +1395,58 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="21">
+      <c r="B21" t="n">
+        <v>-6.0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="n">
+        <v>-7.0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Subclass specific methods implemented
Basically fixed how to get subclass specific attributes, where its not
null if its that class but null in other classes, and added the specific
methods to user, but left empty, and overridden in specific sub classes.
Also added a temporary way to verify someone. Also added test cases for
it and it passes all the tests.
</commit_message>
<xml_diff>
--- a/pdTwo/src/main/resources/csv/user.xlsx
+++ b/pdTwo/src/main/resources/csv/user.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="55">
   <si>
     <t>name</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>helloworld8</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
   </si>
 </sst>
 </file>
@@ -1383,13 +1386,13 @@
         <v>26</v>
       </c>
       <c r="F20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" t="s">
         <v>35</v>
       </c>
       <c r="H20" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="I20" t="n">
         <v>0.0</v>

</xml_diff>

<commit_message>
Partial Implementation of the FacultyTest class and made some updates to the Faculty class
</commit_message>
<xml_diff>
--- a/pdTwo/src/main/resources/csv/user.xlsx
+++ b/pdTwo/src/main/resources/csv/user.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
   <si>
     <t>name</t>
   </si>
@@ -144,6 +144,18 @@
   </si>
   <si>
     <t>Computer Science</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>newfaculty@university.edu</t>
+  </si>
+  <si>
+    <t>newpass</t>
+  </si>
+  <si>
+    <t>Faculty</t>
   </si>
 </sst>
 </file>
@@ -985,32 +997,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A2:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
@@ -1192,6 +1184,32 @@
         <v>35</v>
       </c>
       <c r="I9" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" t="n">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed old userManagement tests from del2
</commit_message>
<xml_diff>
--- a/pdTwo/src/main/resources/csv/user.xlsx
+++ b/pdTwo/src/main/resources/csv/user.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
   <si>
     <t>name</t>
   </si>
@@ -156,6 +156,15 @@
   </si>
   <si>
     <t>Faculty</t>
+  </si>
+  <si>
+    <t>newuser@example.com</t>
+  </si>
+  <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
+    <t>Biology</t>
   </si>
 </sst>
 </file>
@@ -997,32 +1006,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I10"/>
+  <dimension ref="A3:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-    </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>10</v>
@@ -1041,6 +1030,9 @@
       </c>
       <c r="F3" t="b">
         <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1210,6 +1202,32 @@
         <v>25</v>
       </c>
       <c r="I10" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" t="n">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated UserTest, FacultyTest, and related Classes
</commit_message>
<xml_diff>
--- a/pdTwo/src/main/resources/csv/user.xlsx
+++ b/pdTwo/src/main/resources/csv/user.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="44">
   <si>
     <t>name</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Biology</t>
+  </si>
+  <si>
+    <t>Physics</t>
   </si>
 </sst>
 </file>

</xml_diff>